<commit_message>
expand data from 2015
</commit_message>
<xml_diff>
--- a/descstatistics.xlsx
+++ b/descstatistics.xlsx
@@ -1,21 +1,128 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bc2f1dc68cd9768/ukrain war/ukrainn war/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_51CC3ED68F79A8D366075C52F37BD2725ACF81B8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51E83562-A1E1-4F55-A434-B92EF6940291}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>rownames(desc)</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>skew</t>
+  </si>
+  <si>
+    <t>kurt</t>
+  </si>
+  <si>
+    <t>BVSP.Close</t>
+  </si>
+  <si>
+    <t>JKII.Close</t>
+  </si>
+  <si>
+    <t>NG.F.Close</t>
+  </si>
+  <si>
+    <t>N225.Close</t>
+  </si>
+  <si>
+    <t>NSEI.Close</t>
+  </si>
+  <si>
+    <t>XU100.IS.Close</t>
+  </si>
+  <si>
+    <t>X000001.SS.Close</t>
+  </si>
+  <si>
+    <t>BTC.USD.Close</t>
+  </si>
+  <si>
+    <t>FCHI.Close</t>
+  </si>
+  <si>
+    <t>SI.F.Close</t>
+  </si>
+  <si>
+    <t>FTSEMIB.MI.Close</t>
+  </si>
+  <si>
+    <t>FTSE.Close</t>
+  </si>
+  <si>
+    <t>CL.F.Close</t>
+  </si>
+  <si>
+    <t>GSPTSE.Close</t>
+  </si>
+  <si>
+    <t>GDAXI.Close</t>
+  </si>
+  <si>
+    <t>M.BA.Close</t>
+  </si>
+  <si>
+    <t>ALI.F.Close</t>
+  </si>
+  <si>
+    <t>GC.F.Close</t>
+  </si>
+  <si>
+    <t>KS11.Close</t>
+  </si>
+  <si>
+    <t>SB.F.Close</t>
+  </si>
+  <si>
+    <t>MXX.Close</t>
+  </si>
+  <si>
+    <t>LTC.USD.Close</t>
+  </si>
+  <si>
+    <t>IMOEX.ME.Close</t>
+  </si>
+  <si>
+    <t>GSPC.Close</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +170,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +256,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +308,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,349 +501,316 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>rownames(desc)</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>sd</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>median</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>min</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>max</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>skew</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>kurt</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>BVSP.Close</t>
-        </is>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>0.0006317949725039174</v>
+        <v>6.4181097181669237E-4</v>
       </c>
       <c r="C2">
-        <v>0.01986589734687033</v>
+        <v>1.9860294783945531E-2</v>
       </c>
       <c r="D2">
-        <v>0.001225422088399597</v>
+        <v>1.228713093322398E-3</v>
       </c>
       <c r="E2">
-        <v>-0.159930265676044</v>
+        <v>-0.15993026567604399</v>
       </c>
       <c r="F2">
-        <v>0.1302228102427083</v>
+        <v>0.13022281024270829</v>
       </c>
       <c r="G2">
-        <v>-0.0138879900027014</v>
+        <v>-1.0624269893203369E-2</v>
       </c>
       <c r="H2">
-        <v>1.367700122005864</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>JKII.Close</t>
-        </is>
+        <v>1.361223182808506</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>-0.0001058893935944667</v>
+        <v>-1.2900686459687411E-4</v>
       </c>
       <c r="C3">
-        <v>0.01550748718180524</v>
+        <v>1.5520871212248769E-2</v>
       </c>
       <c r="D3">
-        <v>0.0002433584335364003</v>
+        <v>1.8431275166097549E-4</v>
       </c>
       <c r="E3">
-        <v>-0.1285453381957229</v>
+        <v>-0.12854533819572289</v>
       </c>
       <c r="F3">
-        <v>0.08893648578197322</v>
+        <v>8.8936485781973218E-2</v>
       </c>
       <c r="G3">
-        <v>0.01345132919502164</v>
+        <v>2.02828767661083E-2</v>
       </c>
       <c r="H3">
-        <v>1.457963359559042</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>NG.F.Close</t>
-        </is>
+        <v>1.4609148443203821</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>0.000681409934979628</v>
+        <v>6.918854222432994E-4</v>
       </c>
       <c r="C4">
-        <v>0.04197951082650835</v>
+        <v>4.1962980998394607E-2</v>
       </c>
       <c r="D4">
-        <v>-0.0003686635986455134</v>
+        <v>-3.5713290696992578E-4</v>
       </c>
       <c r="E4">
-        <v>-0.300479762578425</v>
+        <v>-0.30047976257842501</v>
       </c>
       <c r="F4">
         <v>0.4355212407018601</v>
       </c>
       <c r="G4">
-        <v>0.02039817345530282</v>
+        <v>1.980234896347139E-2</v>
       </c>
       <c r="H4">
-        <v>1.344465444705103</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>N225.Close</t>
-        </is>
+        <v>1.344859489447356</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>0.0004127240143610823</v>
+        <v>3.9699575886145358E-4</v>
       </c>
       <c r="C5">
-        <v>0.01537270240778184</v>
+        <v>1.5375458650989011E-2</v>
       </c>
       <c r="D5">
-        <v>0.0003689342777324356</v>
+        <v>3.5810780858547281E-4</v>
       </c>
       <c r="E5">
-        <v>-0.0825293281087145</v>
+        <v>-8.2529328108714495E-2</v>
       </c>
       <c r="F5">
         <v>0.1200715718075074</v>
       </c>
       <c r="G5">
-        <v>0.03122360141926218</v>
+        <v>3.0624467850322919E-2</v>
       </c>
       <c r="H5">
-        <v>1.616862806793267</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>NSEI.Close</t>
-        </is>
+        <v>1.6218363906397739</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>0.0005588139172607276</v>
+        <v>5.3903645869831849E-4</v>
       </c>
       <c r="C6">
-        <v>0.01312694979587826</v>
+        <v>1.3138643052969559E-2</v>
       </c>
       <c r="D6">
-        <v>0.0007980423048170593</v>
+        <v>7.934454475106989E-4</v>
       </c>
       <c r="E6">
-        <v>-0.1045383210999589</v>
+        <v>-0.10453832109995891</v>
       </c>
       <c r="F6">
-        <v>0.08400295208862119</v>
+        <v>8.4002952088621186E-2</v>
       </c>
       <c r="G6">
-        <v>0.04317781130335888</v>
+        <v>4.0266086855992561E-2</v>
       </c>
       <c r="H6">
-        <v>1.386762090386065</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>XU100.IS.Close</t>
-        </is>
+        <v>1.384160927541398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>-0.003072153680847165</v>
+        <v>-3.0918226787584281E-3</v>
       </c>
       <c r="C7">
-        <v>0.1359339412685209</v>
+        <v>0.13587714470600989</v>
       </c>
       <c r="D7">
-        <v>0.001940994428344389</v>
+        <v>1.936356920683391E-3</v>
       </c>
       <c r="E7">
-        <v>-4.592629753776787</v>
+        <v>-4.5926297537767873</v>
       </c>
       <c r="F7">
         <v>0.1081991258551796</v>
       </c>
       <c r="G7">
-        <v>-0.08938923557993404</v>
+        <v>-8.995475410326384E-2</v>
       </c>
       <c r="H7">
-        <v>1.42361168225257</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>X000001.SS.Close</t>
-        </is>
+        <v>1.4236813330111711</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>-8.665408423720353e-005</v>
+        <v>-8.7622299845267236E-5</v>
       </c>
       <c r="C8">
-        <v>0.01744337797720506</v>
+        <v>1.7435908353049121E-2</v>
       </c>
       <c r="D8">
-        <v>0.0005464156421037814</v>
+        <v>5.2571217952479543E-4</v>
       </c>
       <c r="E8">
         <v>-0.106284707595627</v>
       </c>
       <c r="F8">
-        <v>0.1004530633650429</v>
+        <v>0.10045306336504289</v>
       </c>
       <c r="G8">
-        <v>-0.05680504057571004</v>
+        <v>-5.4005336028561467E-2</v>
       </c>
       <c r="H8">
-        <v>1.684189574995316</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>BTC.USD.Close</t>
-        </is>
+        <v>1.68541508857789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>0.00424066341351826</v>
+        <v>4.2403211903344574E-3</v>
       </c>
       <c r="C9">
-        <v>0.05867721112617237</v>
+        <v>5.865198020324041E-2</v>
       </c>
       <c r="D9">
-        <v>0.00294957259491202</v>
+        <v>2.966396215320799E-3</v>
       </c>
       <c r="E9">
-        <v>-0.4647301753548501</v>
+        <v>-0.46473017535485012</v>
       </c>
       <c r="F9">
-        <v>0.2706375177187859</v>
+        <v>0.27063751771878591</v>
       </c>
       <c r="G9">
-        <v>0.1017138874017027</v>
+        <v>0.10047862998039279</v>
       </c>
       <c r="H9">
-        <v>1.834753577721529</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>FCHI.Close</t>
-        </is>
+        <v>1.835699998947991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>0.0003253189116862709</v>
+        <v>3.1629813432089828E-4</v>
       </c>
       <c r="C10">
-        <v>0.01568123731169237</v>
+        <v>1.5677515315859449E-2</v>
       </c>
       <c r="D10">
-        <v>0.0008982699817909889</v>
+        <v>8.9681522410423042E-4</v>
       </c>
       <c r="E10">
         <v>-0.1309834911294932</v>
       </c>
       <c r="F10">
-        <v>0.1642145644457109</v>
+        <v>0.16421456444571089</v>
       </c>
       <c r="G10">
-        <v>-0.00889770137809918</v>
+        <v>-1.1882609484893459E-2</v>
       </c>
       <c r="H10">
-        <v>1.561556911396751</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>SI.F.Close</t>
-        </is>
+        <v>1.5582696740092641</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>0.0001650803230807161</v>
+        <v>1.3272868108386041E-4</v>
       </c>
       <c r="C11">
-        <v>0.02157250311249393</v>
+        <v>2.1591457054416011E-2</v>
       </c>
       <c r="D11">
-        <v>0.0001751978279949107</v>
+        <v>1.6501927096013169E-4</v>
       </c>
       <c r="E11">
-        <v>-0.1607706392886614</v>
+        <v>-0.16077063928866139</v>
       </c>
       <c r="F11">
         <v>0.1908000205554545</v>
       </c>
       <c r="G11">
-        <v>0.007114245928477046</v>
+        <v>7.0949606402026634E-3</v>
       </c>
       <c r="H11">
-        <v>1.442113011019511</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>FTSEMIB.MI.Close</t>
-        </is>
+        <v>1.441602289346541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
       </c>
       <c r="B12">
-        <v>0.0001942102000533327</v>
+        <v>1.8830263228238251E-4</v>
       </c>
       <c r="C12">
-        <v>0.01798836513393227</v>
+        <v>1.7981759458506389E-2</v>
       </c>
       <c r="D12">
-        <v>0.0008349630244914863</v>
+        <v>8.3167454987620459E-4</v>
       </c>
       <c r="E12">
         <v>-0.1854610663248373</v>
@@ -701,163 +819,151 @@
         <v>0.1159782860158725</v>
       </c>
       <c r="G12">
-        <v>-0.04172333868132191</v>
+        <v>-4.0699112175105447E-2</v>
       </c>
       <c r="H12">
-        <v>1.55269359490486</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>FTSE.Close</t>
-        </is>
+        <v>1.5550917691511821</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
       </c>
       <c r="B13">
-        <v>0.0001012162421556027</v>
+        <v>8.7648162043621101E-5</v>
       </c>
       <c r="C13">
-        <v>0.01287717442029588</v>
+        <v>1.287995823510197E-2</v>
       </c>
       <c r="D13">
-        <v>0.0003650951383473711</v>
+        <v>3.633900059272222E-4</v>
       </c>
       <c r="E13">
         <v>-0.1151170613425148</v>
       </c>
       <c r="F13">
-        <v>0.1212538255279725</v>
+        <v>0.12125382552797249</v>
       </c>
       <c r="G13">
-        <v>0.01213268792166887</v>
+        <v>9.6041153887672023E-3</v>
       </c>
       <c r="H13">
-        <v>1.40049653335595</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>CL.F.Close</t>
-        </is>
+        <v>1.4035827338729021</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
       </c>
       <c r="B14">
-        <v>0.0009090867940400866</v>
+        <v>9.1171235795051836E-4</v>
       </c>
       <c r="C14">
-        <v>0.04229295257486954</v>
+        <v>4.2274860872317681E-2</v>
       </c>
       <c r="D14">
-        <v>0.002327886005748958</v>
+        <v>2.374800994116022E-3</v>
       </c>
       <c r="E14">
-        <v>-0.2817962993063952</v>
+        <v>-0.28179629930639521</v>
       </c>
       <c r="F14">
         <v>0.7367530178235584</v>
       </c>
       <c r="G14">
-        <v>-0.1113115025375462</v>
+        <v>-0.1147674834513133</v>
       </c>
       <c r="H14">
-        <v>1.498823567174011</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>GSPTSE.Close</t>
-        </is>
+        <v>1.503677582008248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
       </c>
       <c r="B15">
-        <v>0.0002851702008216192</v>
+        <v>2.7891909782788059E-4</v>
       </c>
       <c r="C15">
-        <v>0.01175886144788862</v>
+        <v>1.1755739697853731E-2</v>
       </c>
       <c r="D15">
-        <v>0.0008626582239852354</v>
+        <v>8.5292569224471038E-4</v>
       </c>
       <c r="E15">
         <v>-0.1317579985597099</v>
       </c>
       <c r="F15">
-        <v>0.09408816405878362</v>
+        <v>9.4088164058783619E-2</v>
       </c>
       <c r="G15">
-        <v>-0.05416776493399141</v>
+        <v>-5.3435991757440592E-2</v>
       </c>
       <c r="H15">
-        <v>1.464015366282281</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>GDAXI.Close</t>
-        </is>
+        <v>1.462156157226336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
       </c>
       <c r="B16">
-        <v>0.0002816440920966532</v>
+        <v>2.758551208148665E-4</v>
       </c>
       <c r="C16">
-        <v>0.01553250619208246</v>
+        <v>1.552708316493559E-2</v>
       </c>
       <c r="D16">
-        <v>0.0007726518282868966</v>
+        <v>7.6771240372597305E-4</v>
       </c>
       <c r="E16">
-        <v>-0.1305485870386605</v>
+        <v>-0.13054858703866051</v>
       </c>
       <c r="F16">
-        <v>0.1497068616012669</v>
+        <v>0.14970686160126689</v>
       </c>
       <c r="G16">
-        <v>-0.01124163359045094</v>
+        <v>-1.637117992318628E-2</v>
       </c>
       <c r="H16">
-        <v>1.621952013830478</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>M.BA.Close</t>
-        </is>
+        <v>1.6107497941705251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
       </c>
       <c r="B17">
-        <v>0.001952506943178072</v>
+        <v>1.948401777338781E-3</v>
       </c>
       <c r="C17">
-        <v>0.03154189518427005</v>
+        <v>3.1528642780562513E-2</v>
       </c>
       <c r="D17">
-        <v>0.001922836649645987</v>
+        <v>1.912507921731255E-3</v>
       </c>
       <c r="E17">
-        <v>-0.3775661201880389</v>
+        <v>-0.37756612018803892</v>
       </c>
       <c r="F17">
-        <v>0.1685137904182774</v>
+        <v>0.16851379041827741</v>
       </c>
       <c r="G17">
-        <v>0.02570809261168939</v>
+        <v>2.5719134488267702E-2</v>
       </c>
       <c r="H17">
-        <v>1.48795239987139</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ALI.F.Close</t>
-        </is>
+        <v>1.488304394283982</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
       </c>
       <c r="B18">
-        <v>0.0001770373779518849</v>
+        <v>1.6485759612083531E-4</v>
       </c>
       <c r="C18">
-        <v>0.01428421565853729</v>
+        <v>1.4284118845206729E-2</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -866,209 +972,195 @@
         <v>-0.2009204145294996</v>
       </c>
       <c r="F18">
-        <v>0.05453994794652317</v>
+        <v>5.4539947946523171E-2</v>
       </c>
       <c r="G18">
-        <v>0.05563376266963745</v>
+        <v>4.7273444042132642E-2</v>
       </c>
       <c r="H18">
-        <v>2.156821596645281</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>GC.F.Close</t>
-        </is>
+        <v>2.149138930623594</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
       </c>
       <c r="B19">
-        <v>0.0003001204841850712</v>
+        <v>2.864023553338685E-4</v>
       </c>
       <c r="C19">
-        <v>0.01146029416715779</v>
+        <v>1.146492309122607E-2</v>
       </c>
       <c r="D19">
-        <v>0.0003897268213295391</v>
+        <v>3.8957505262926523E-4</v>
       </c>
       <c r="E19">
-        <v>-0.05106938390113047</v>
+        <v>-5.1069383901130472E-2</v>
       </c>
       <c r="F19">
         <v>0.1097401996827569</v>
       </c>
       <c r="G19">
-        <v>0.04109373820863316</v>
+        <v>3.925495831851028E-2</v>
       </c>
       <c r="H19">
-        <v>1.50199149450222</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>KS11.Close</t>
-        </is>
+        <v>1.5045774660427489</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
       </c>
       <c r="B20">
-        <v>0.0002808200112437579</v>
+        <v>2.6648151842271648E-4</v>
       </c>
       <c r="C20">
-        <v>0.01266278734914549</v>
+        <v>1.266679201988963E-2</v>
       </c>
       <c r="D20">
-        <v>0.0006608428920591436</v>
+        <v>6.493096308655133E-4</v>
       </c>
       <c r="E20">
-        <v>-0.08766971795460687</v>
+        <v>-8.7669717954606874E-2</v>
       </c>
       <c r="F20">
-        <v>0.1456824924644868</v>
+        <v>0.14568249246448681</v>
       </c>
       <c r="G20">
-        <v>-0.02319782402006621</v>
+        <v>-2.3334706183050911E-2</v>
       </c>
       <c r="H20">
-        <v>1.652471289023971</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>SB.F.Close</t>
-        </is>
+        <v>1.660901130540563</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
       </c>
       <c r="B21">
-        <v>0.0002099192866240111</v>
+        <v>2.138970367766435E-4</v>
       </c>
       <c r="C21">
-        <v>0.02374223113490042</v>
+        <v>2.3732409642701489E-2</v>
       </c>
       <c r="D21">
-        <v>-0.0007797271350211688</v>
+        <v>-7.713973517620154E-4</v>
       </c>
       <c r="E21">
-        <v>-0.09066608466112225</v>
+        <v>-9.0666084661122248E-2</v>
       </c>
       <c r="F21">
-        <v>0.2096167750160078</v>
+        <v>0.20961677501600781</v>
       </c>
       <c r="G21">
-        <v>0.02567763866983925</v>
+        <v>2.496362276688845E-2</v>
       </c>
       <c r="H21">
-        <v>1.302534629222834</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>MXX.Close</t>
-        </is>
+        <v>1.3029618920339241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
       </c>
       <c r="B22">
-        <v>0.0001626574147173078</v>
+        <v>1.630943860011785E-4</v>
       </c>
       <c r="C22">
-        <v>0.01184986727724964</v>
+        <v>1.1844781037878199E-2</v>
       </c>
       <c r="D22">
-        <v>7.21114321375893e-005</v>
+        <v>7.6210148564292979E-5</v>
       </c>
       <c r="E22">
-        <v>-0.06772465680778872</v>
+        <v>-6.7724656807788719E-2</v>
       </c>
       <c r="F22">
-        <v>0.0533584316741802</v>
+        <v>5.3358431674180203E-2</v>
       </c>
       <c r="G22">
-        <v>0.04992941118221572</v>
+        <v>4.9483386713390108E-2</v>
       </c>
       <c r="H22">
-        <v>1.394288081227058</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LTC.USD.Close</t>
-        </is>
+        <v>1.3968202091250721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
       </c>
       <c r="B23">
-        <v>0.003334225077035469</v>
+        <v>3.30526775766122E-3</v>
       </c>
       <c r="C23">
-        <v>0.08780488352070791</v>
+        <v>8.7772686344256251E-2</v>
       </c>
       <c r="D23">
-        <v>0.0003289806879216428</v>
+        <v>3.2252145979017039E-4</v>
       </c>
       <c r="E23">
-        <v>-0.4490616421000784</v>
+        <v>-0.44906164210007837</v>
       </c>
       <c r="F23">
-        <v>0.7789774982240303</v>
+        <v>0.77897749822403028</v>
       </c>
       <c r="G23">
-        <v>0.01379752813673451</v>
+        <v>8.7115819963108163E-3</v>
       </c>
       <c r="H23">
-        <v>2.017967521725502</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>IMOEX.ME.Close</t>
-        </is>
+        <v>2.0075911806195732</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
       </c>
       <c r="B24">
-        <v>0.0003356946625425855</v>
+        <v>3.0267027895422327E-4</v>
       </c>
       <c r="C24">
-        <v>0.0201533555878399</v>
+        <v>2.017617353689825E-2</v>
       </c>
       <c r="D24">
-        <v>0.0007580593513729639</v>
+        <v>7.3266211479383614E-4</v>
       </c>
       <c r="E24">
-        <v>-0.4046743701978492</v>
+        <v>-0.40467437019784919</v>
       </c>
       <c r="F24">
-        <v>0.1826194540502364</v>
+        <v>0.18261945405023641</v>
       </c>
       <c r="G24">
-        <v>0.01752958129788561</v>
+        <v>2.0764290722470439E-2</v>
       </c>
       <c r="H24">
-        <v>1.315260533756243</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>GSPC.Close</t>
-        </is>
+        <v>1.312655220115341</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
       </c>
       <c r="B25">
-        <v>0.0005964513360951461</v>
+        <v>5.9482482711461571E-4</v>
       </c>
       <c r="C25">
-        <v>0.01309604858260344</v>
+        <v>1.3090534704161969E-2</v>
       </c>
       <c r="D25">
-        <v>0.0009831508870483674</v>
+        <v>9.6829259383124366E-4</v>
       </c>
       <c r="E25">
-        <v>-0.09994485230080308</v>
+        <v>-9.9944852300803078E-2</v>
       </c>
       <c r="F25">
-        <v>0.08880840695207493</v>
+        <v>8.8808406952074925E-2</v>
       </c>
       <c r="G25">
-        <v>0.05689537055366919</v>
+        <v>6.0616666989335523E-2</v>
       </c>
       <c r="H25">
-        <v>1.656547525913391</v>
+        <v>1.659082727578322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding commodities and 3 major crypto
</commit_message>
<xml_diff>
--- a/descstatistics.xlsx
+++ b/descstatistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bc2f1dc68cd9768/ukrain war/ukrainn war/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_51CC3ED68F79A8D366075C52F37BD2725ACF81B8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51E83562-A1E1-4F55-A434-B92EF6940291}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_D5501DDC8F79A8D366075C52F37BD2725AC67C55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2F7D2F5-0B7A-4E93-A4C7-1C76DD06C79D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>rownames(desc)</t>
   </si>
@@ -46,76 +46,79 @@
     <t>kurt</t>
   </si>
   <si>
-    <t>BVSP.Close</t>
-  </si>
-  <si>
-    <t>JKII.Close</t>
-  </si>
-  <si>
-    <t>NG.F.Close</t>
-  </si>
-  <si>
-    <t>N225.Close</t>
-  </si>
-  <si>
-    <t>NSEI.Close</t>
-  </si>
-  <si>
-    <t>XU100.IS.Close</t>
-  </si>
-  <si>
-    <t>X000001.SS.Close</t>
-  </si>
-  <si>
-    <t>BTC.USD.Close</t>
-  </si>
-  <si>
-    <t>FCHI.Close</t>
-  </si>
-  <si>
-    <t>SI.F.Close</t>
-  </si>
-  <si>
-    <t>FTSEMIB.MI.Close</t>
-  </si>
-  <si>
-    <t>FTSE.Close</t>
-  </si>
-  <si>
-    <t>CL.F.Close</t>
-  </si>
-  <si>
-    <t>GSPTSE.Close</t>
-  </si>
-  <si>
-    <t>GDAXI.Close</t>
-  </si>
-  <si>
-    <t>M.BA.Close</t>
-  </si>
-  <si>
-    <t>ALI.F.Close</t>
-  </si>
-  <si>
-    <t>GC.F.Close</t>
-  </si>
-  <si>
-    <t>KS11.Close</t>
-  </si>
-  <si>
-    <t>SB.F.Close</t>
-  </si>
-  <si>
-    <t>MXX.Close</t>
-  </si>
-  <si>
-    <t>LTC.USD.Close</t>
-  </si>
-  <si>
-    <t>IMOEX.ME.Close</t>
-  </si>
-  <si>
-    <t>GSPC.Close</t>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>Soybean</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Bitcoin</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Agentina</t>
+  </si>
+  <si>
+    <t>corn</t>
+  </si>
+  <si>
+    <t>Aluminium</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Southkorea</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -502,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -544,10 +547,10 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>6.4181097181669237E-4</v>
+        <v>6.4291563786112739E-4</v>
       </c>
       <c r="C2">
-        <v>1.9860294783945531E-2</v>
+        <v>1.9880649303973451E-2</v>
       </c>
       <c r="D2">
         <v>1.228713093322398E-3</v>
@@ -559,10 +562,10 @@
         <v>0.13022281024270829</v>
       </c>
       <c r="G2">
-        <v>-1.0624269893203369E-2</v>
+        <v>-9.7951629429315658E-3</v>
       </c>
       <c r="H2">
-        <v>1.361223182808506</v>
+        <v>1.3689235482710871</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -570,10 +573,10 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>-1.2900686459687411E-4</v>
+        <v>-1.2922890739308209E-4</v>
       </c>
       <c r="C3">
-        <v>1.5520871212248769E-2</v>
+        <v>1.5517287597128129E-2</v>
       </c>
       <c r="D3">
         <v>1.8431275166097549E-4</v>
@@ -585,10 +588,10 @@
         <v>8.8936485781973218E-2</v>
       </c>
       <c r="G3">
-        <v>2.02828767661083E-2</v>
+        <v>2.0953543744132629E-2</v>
       </c>
       <c r="H3">
-        <v>1.4609148443203821</v>
+        <v>1.450714907252513</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -596,10 +599,10 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>6.918854222432994E-4</v>
+        <v>6.9307627494939804E-4</v>
       </c>
       <c r="C4">
-        <v>4.1962980998394607E-2</v>
+        <v>4.1856606030690503E-2</v>
       </c>
       <c r="D4">
         <v>-3.5713290696992578E-4</v>
@@ -611,10 +614,10 @@
         <v>0.4355212407018601</v>
       </c>
       <c r="G4">
-        <v>1.980234896347139E-2</v>
+        <v>1.977174054883293E-2</v>
       </c>
       <c r="H4">
-        <v>1.344859489447356</v>
+        <v>1.342815844242139</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -622,25 +625,25 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>3.9699575886145358E-4</v>
+        <v>4.4109583137454209E-4</v>
       </c>
       <c r="C5">
-        <v>1.5375458650989011E-2</v>
+        <v>1.614095492849545E-2</v>
       </c>
       <c r="D5">
-        <v>3.5810780858547281E-4</v>
+        <v>7.8435731095716221E-4</v>
       </c>
       <c r="E5">
-        <v>-8.2529328108714495E-2</v>
+        <v>-9.6032648614778005E-2</v>
       </c>
       <c r="F5">
-        <v>0.1200715718075074</v>
+        <v>7.6889340761719716E-2</v>
       </c>
       <c r="G5">
-        <v>3.0624467850322919E-2</v>
+        <v>-6.4504818187804208E-2</v>
       </c>
       <c r="H5">
-        <v>1.6218363906397739</v>
+        <v>1.4156451595634061</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -648,25 +651,25 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>5.3903645869831849E-4</v>
+        <v>3.9767905620889161E-4</v>
       </c>
       <c r="C6">
-        <v>1.3138643052969559E-2</v>
+        <v>1.5386495198442681E-2</v>
       </c>
       <c r="D6">
-        <v>7.934454475106989E-4</v>
+        <v>3.5810780858547281E-4</v>
       </c>
       <c r="E6">
-        <v>-0.10453832109995891</v>
+        <v>-8.2529328108714495E-2</v>
       </c>
       <c r="F6">
-        <v>8.4002952088621186E-2</v>
+        <v>0.1200715718075074</v>
       </c>
       <c r="G6">
-        <v>4.0266086855992561E-2</v>
+        <v>3.2334377773556043E-2</v>
       </c>
       <c r="H6">
-        <v>1.384160927541398</v>
+        <v>1.6169321173679649</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -674,25 +677,25 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>-3.0918226787584281E-3</v>
+        <v>5.3996423229332421E-4</v>
       </c>
       <c r="C7">
-        <v>0.13587714470600989</v>
+        <v>1.3154207050609081E-2</v>
       </c>
       <c r="D7">
-        <v>1.936356920683391E-3</v>
+        <v>7.7750118615593777E-4</v>
       </c>
       <c r="E7">
-        <v>-4.5926297537767873</v>
+        <v>-0.10453832109995891</v>
       </c>
       <c r="F7">
-        <v>0.1081991258551796</v>
+        <v>8.4002952088621186E-2</v>
       </c>
       <c r="G7">
-        <v>-8.995475410326384E-2</v>
+        <v>4.202300770608166E-2</v>
       </c>
       <c r="H7">
-        <v>1.4236813330111711</v>
+        <v>1.3888611574316829</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -700,25 +703,25 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>-8.7622299845267236E-5</v>
+        <v>-3.097144232422383E-3</v>
       </c>
       <c r="C8">
-        <v>1.7435908353049121E-2</v>
+        <v>0.135994192365678</v>
       </c>
       <c r="D8">
-        <v>5.2571217952479543E-4</v>
+        <v>1.936356920683391E-3</v>
       </c>
       <c r="E8">
-        <v>-0.106284707595627</v>
+        <v>-4.5926297537767873</v>
       </c>
       <c r="F8">
-        <v>0.10045306336504289</v>
+        <v>0.1081991258551796</v>
       </c>
       <c r="G8">
-        <v>-5.4005336028561467E-2</v>
+        <v>-9.0520017655510099E-2</v>
       </c>
       <c r="H8">
-        <v>1.68541508857789</v>
+        <v>1.4367808854469539</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -726,25 +729,25 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>4.2403211903344574E-3</v>
+        <v>-8.777311275377889E-5</v>
       </c>
       <c r="C9">
-        <v>5.865198020324041E-2</v>
+        <v>1.7453704370625159E-2</v>
       </c>
       <c r="D9">
-        <v>2.966396215320799E-3</v>
+        <v>5.2571217952479543E-4</v>
       </c>
       <c r="E9">
-        <v>-0.46473017535485012</v>
+        <v>-0.106284707595627</v>
       </c>
       <c r="F9">
-        <v>0.27063751771878591</v>
+        <v>0.10045306336504289</v>
       </c>
       <c r="G9">
-        <v>0.10047862998039279</v>
+        <v>-5.207946944486818E-2</v>
       </c>
       <c r="H9">
-        <v>1.835699998947991</v>
+        <v>1.691730993499833</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -752,25 +755,25 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>3.1629813432089828E-4</v>
+        <v>4.2476195056362371E-3</v>
       </c>
       <c r="C10">
-        <v>1.5677515315859449E-2</v>
+        <v>5.8782359894833748E-2</v>
       </c>
       <c r="D10">
-        <v>8.9681522410423042E-4</v>
+        <v>2.8668584817119762E-3</v>
       </c>
       <c r="E10">
-        <v>-0.1309834911294932</v>
+        <v>-0.46473017535485012</v>
       </c>
       <c r="F10">
-        <v>0.16421456444571089</v>
+        <v>0.27063751771878591</v>
       </c>
       <c r="G10">
-        <v>-1.1882609484893459E-2</v>
+        <v>0.1038063957261643</v>
       </c>
       <c r="H10">
-        <v>1.5582696740092641</v>
+        <v>1.8436114542407069</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -778,25 +781,25 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>1.3272868108386041E-4</v>
+        <v>3.168425373059601E-4</v>
       </c>
       <c r="C11">
-        <v>2.1591457054416011E-2</v>
+        <v>1.5691293395543648E-2</v>
       </c>
       <c r="D11">
-        <v>1.6501927096013169E-4</v>
+        <v>8.9681522410423042E-4</v>
       </c>
       <c r="E11">
-        <v>-0.16077063928866139</v>
+        <v>-0.1309834911294932</v>
       </c>
       <c r="F11">
-        <v>0.1908000205554545</v>
+        <v>0.16421456444571089</v>
       </c>
       <c r="G11">
-        <v>7.0949606402026634E-3</v>
+        <v>-8.6352972069750327E-3</v>
       </c>
       <c r="H11">
-        <v>1.441602289346541</v>
+        <v>1.566487066991447</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,13 +807,13 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>1.8830263228238251E-4</v>
+        <v>1.8862673319853119E-4</v>
       </c>
       <c r="C12">
-        <v>1.7981759458506389E-2</v>
+        <v>1.7987949396026819E-2</v>
       </c>
       <c r="D12">
-        <v>8.3167454987620459E-4</v>
+        <v>8.4292293336130086E-4</v>
       </c>
       <c r="E12">
         <v>-0.1854610663248373</v>
@@ -819,10 +822,10 @@
         <v>0.1159782860158725</v>
       </c>
       <c r="G12">
-        <v>-4.0699112175105447E-2</v>
+        <v>-3.9869505430348347E-2</v>
       </c>
       <c r="H12">
-        <v>1.5550917691511821</v>
+        <v>1.5635923156959659</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -830,10 +833,10 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>8.7648162043621101E-5</v>
+        <v>8.7799019465382923E-5</v>
       </c>
       <c r="C13">
-        <v>1.287995823510197E-2</v>
+        <v>1.288502680745753E-2</v>
       </c>
       <c r="D13">
         <v>3.633900059272222E-4</v>
@@ -845,10 +848,10 @@
         <v>0.12125382552797249</v>
       </c>
       <c r="G13">
-        <v>9.6041153887672023E-3</v>
+        <v>1.122482789143861E-2</v>
       </c>
       <c r="H13">
-        <v>1.4035827338729021</v>
+        <v>1.4039457700838089</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -856,10 +859,10 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>9.1171235795051836E-4</v>
+        <v>9.1328157027057094E-4</v>
       </c>
       <c r="C14">
-        <v>4.2274860872317681E-2</v>
+        <v>4.2308907853507188E-2</v>
       </c>
       <c r="D14">
         <v>2.374800994116022E-3</v>
@@ -871,10 +874,10 @@
         <v>0.7367530178235584</v>
       </c>
       <c r="G14">
-        <v>-0.1147674834513133</v>
+        <v>-0.11513397737182179</v>
       </c>
       <c r="H14">
-        <v>1.503677582008248</v>
+        <v>1.5161191214833429</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -882,10 +885,10 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>2.7891909782788059E-4</v>
+        <v>2.7939916512190448E-4</v>
       </c>
       <c r="C15">
-        <v>1.1755739697853731E-2</v>
+        <v>1.1771010532707271E-2</v>
       </c>
       <c r="D15">
         <v>8.5292569224471038E-4</v>
@@ -897,10 +900,10 @@
         <v>9.4088164058783619E-2</v>
       </c>
       <c r="G15">
-        <v>-5.3435991757440592E-2</v>
+        <v>-5.1615837304885538E-2</v>
       </c>
       <c r="H15">
-        <v>1.462156157226336</v>
+        <v>1.461663009470425</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -908,10 +911,10 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>2.758551208148665E-4</v>
+        <v>2.7632991448236192E-4</v>
       </c>
       <c r="C16">
-        <v>1.552708316493559E-2</v>
+        <v>1.554033383118867E-2</v>
       </c>
       <c r="D16">
         <v>7.6771240372597305E-4</v>
@@ -923,10 +926,10 @@
         <v>0.14970686160126689</v>
       </c>
       <c r="G16">
-        <v>-1.637117992318628E-2</v>
+        <v>-1.687711781677995E-2</v>
       </c>
       <c r="H16">
-        <v>1.6107497941705251</v>
+        <v>1.6114534569604659</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,10 +937,10 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>1.948401777338781E-3</v>
+        <v>1.951755308797196E-3</v>
       </c>
       <c r="C17">
-        <v>3.1528642780562513E-2</v>
+        <v>3.1552103605129792E-2</v>
       </c>
       <c r="D17">
         <v>1.912507921731255E-3</v>
@@ -949,10 +952,10 @@
         <v>0.16851379041827741</v>
       </c>
       <c r="G17">
-        <v>2.5719134488267702E-2</v>
+        <v>2.7151174614956801E-2</v>
       </c>
       <c r="H17">
-        <v>1.488304394283982</v>
+        <v>1.4877762903375309</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -960,25 +963,25 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>1.6485759612083531E-4</v>
+        <v>6.5212655517716124E-4</v>
       </c>
       <c r="C18">
-        <v>1.4284118845206729E-2</v>
+        <v>1.999312739375626E-2</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1.3571869974233759E-3</v>
       </c>
       <c r="E18">
-        <v>-0.2009204145294996</v>
+        <v>-0.2057265653202078</v>
       </c>
       <c r="F18">
-        <v>5.4539947946523171E-2</v>
+        <v>0.1339103958505872</v>
       </c>
       <c r="G18">
-        <v>4.7273444042132642E-2</v>
+        <v>-6.1795955488469008E-2</v>
       </c>
       <c r="H18">
-        <v>2.149138930623594</v>
+        <v>1.35839218371773</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -986,25 +989,25 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>2.864023553338685E-4</v>
+        <v>1.6514134413481271E-4</v>
       </c>
       <c r="C19">
-        <v>1.146492309122607E-2</v>
+        <v>1.4296415200231409E-2</v>
       </c>
       <c r="D19">
-        <v>3.8957505262926523E-4</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>-5.1069383901130472E-2</v>
+        <v>-0.2009204145294996</v>
       </c>
       <c r="F19">
-        <v>0.1097401996827569</v>
+        <v>5.4539947946523171E-2</v>
       </c>
       <c r="G19">
-        <v>3.925495831851028E-2</v>
+        <v>3.9493705548103109E-2</v>
       </c>
       <c r="H19">
-        <v>1.5045774660427489</v>
+        <v>2.1294781255765618</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1012,25 +1015,25 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>2.6648151842271648E-4</v>
+        <v>6.4804182794746127E-4</v>
       </c>
       <c r="C20">
-        <v>1.266679201988963E-2</v>
+        <v>2.390687018478483E-2</v>
       </c>
       <c r="D20">
-        <v>6.493096308655133E-4</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>-8.7669717954606874E-2</v>
+        <v>-9.2255489394731605E-2</v>
       </c>
       <c r="F20">
-        <v>0.14568249246448681</v>
+        <v>0.2252276481622868</v>
       </c>
       <c r="G20">
-        <v>-2.3334706183050911E-2</v>
+        <v>-3.4669312918279359E-3</v>
       </c>
       <c r="H20">
-        <v>1.660901130540563</v>
+        <v>1.313464854523307</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1038,25 +1041,25 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>2.138970367766435E-4</v>
+        <v>2.8689530258917638E-4</v>
       </c>
       <c r="C21">
-        <v>2.3732409642701489E-2</v>
+        <v>1.147740180107438E-2</v>
       </c>
       <c r="D21">
-        <v>-7.713973517620154E-4</v>
+        <v>3.8183038284156368E-4</v>
       </c>
       <c r="E21">
-        <v>-9.0666084661122248E-2</v>
+        <v>-5.1069383901130472E-2</v>
       </c>
       <c r="F21">
-        <v>0.20961677501600781</v>
+        <v>0.1097401996827569</v>
       </c>
       <c r="G21">
-        <v>2.496362276688845E-2</v>
+        <v>3.9568332716219637E-2</v>
       </c>
       <c r="H21">
-        <v>1.3029618920339241</v>
+        <v>1.507395719439995</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1064,25 +1067,25 @@
         <v>28</v>
       </c>
       <c r="B22">
-        <v>1.630943860011785E-4</v>
+        <v>2.6694017852327197E-4</v>
       </c>
       <c r="C22">
-        <v>1.1844781037878199E-2</v>
+        <v>1.267551669990183E-2</v>
       </c>
       <c r="D22">
-        <v>7.6210148564292979E-5</v>
+        <v>6.493096308655133E-4</v>
       </c>
       <c r="E22">
-        <v>-6.7724656807788719E-2</v>
+        <v>-8.7669717954606874E-2</v>
       </c>
       <c r="F22">
-        <v>5.3358431674180203E-2</v>
+        <v>0.14568249246448681</v>
       </c>
       <c r="G22">
-        <v>4.9483386713390108E-2</v>
+        <v>-2.6806533993861011E-2</v>
       </c>
       <c r="H22">
-        <v>1.3968202091250721</v>
+        <v>1.6666184712153289</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1090,25 +1093,25 @@
         <v>29</v>
       </c>
       <c r="B23">
-        <v>3.30526775766122E-3</v>
+        <v>2.1426519002410761E-4</v>
       </c>
       <c r="C23">
-        <v>8.7772686344256251E-2</v>
+        <v>2.3745949189304501E-2</v>
       </c>
       <c r="D23">
-        <v>3.2252145979017039E-4</v>
+        <v>-7.713973517620154E-4</v>
       </c>
       <c r="E23">
-        <v>-0.44906164210007837</v>
+        <v>-9.0666084661122248E-2</v>
       </c>
       <c r="F23">
-        <v>0.77897749822403028</v>
+        <v>0.20961677501600781</v>
       </c>
       <c r="G23">
-        <v>8.7115819963108163E-3</v>
+        <v>2.424096449397363E-2</v>
       </c>
       <c r="H23">
-        <v>2.0075911806195732</v>
+        <v>1.30449133333454</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1116,25 +1119,25 @@
         <v>30</v>
       </c>
       <c r="B24">
-        <v>3.0267027895422327E-4</v>
+        <v>1.633750992300962E-4</v>
       </c>
       <c r="C24">
-        <v>2.017617353689825E-2</v>
+        <v>1.1822394753171921E-2</v>
       </c>
       <c r="D24">
-        <v>7.3266211479383614E-4</v>
+        <v>7.6210148564292979E-5</v>
       </c>
       <c r="E24">
-        <v>-0.40467437019784919</v>
+        <v>-6.7724656807788719E-2</v>
       </c>
       <c r="F24">
-        <v>0.18261945405023641</v>
+        <v>5.3358431674180203E-2</v>
       </c>
       <c r="G24">
-        <v>2.0764290722470439E-2</v>
+        <v>4.3033475798792721E-2</v>
       </c>
       <c r="H24">
-        <v>1.312655220115341</v>
+        <v>1.4047033797279711</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1142,25 +1145,51 @@
         <v>31</v>
       </c>
       <c r="B25">
-        <v>5.9482482711461571E-4</v>
+        <v>3.0319122607806877E-4</v>
       </c>
       <c r="C25">
-        <v>1.3090534704161969E-2</v>
+        <v>2.0193004205695999E-2</v>
       </c>
       <c r="D25">
-        <v>9.6829259383124366E-4</v>
+        <v>7.3266211479383614E-4</v>
       </c>
       <c r="E25">
+        <v>-0.40467437019784919</v>
+      </c>
+      <c r="F25">
+        <v>0.18261945405023641</v>
+      </c>
+      <c r="G25">
+        <v>2.09776731479367E-2</v>
+      </c>
+      <c r="H25">
+        <v>1.3112489957093729</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>5.9584862199777344E-4</v>
+      </c>
+      <c r="C26">
+        <v>1.3122969509003501E-2</v>
+      </c>
+      <c r="D26">
+        <v>9.957057144278636E-4</v>
+      </c>
+      <c r="E26">
         <v>-9.9944852300803078E-2</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>8.8808406952074925E-2</v>
       </c>
-      <c r="G25">
-        <v>6.0616666989335523E-2</v>
-      </c>
-      <c r="H25">
-        <v>1.659082727578322</v>
+      <c r="G26">
+        <v>5.7899481914231658E-2</v>
+      </c>
+      <c r="H26">
+        <v>1.6509950343277391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set connectedness between markets
</commit_message>
<xml_diff>
--- a/descstatistics.xlsx
+++ b/descstatistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0bc2f1dc68cd9768/ukrain war/ukrainn war/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_D5501DDC8F79A8D366075C52F37BD2725AC67C55" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2F7D2F5-0B7A-4E93-A4C7-1C76DD06C79D}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_0B56FED58F79A8D366075C52F37BD2720A456D4D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C27CF9-14AC-49E7-B4C9-B652D9E03E68}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>rownames(desc)</t>
   </si>
@@ -52,7 +52,7 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>NG</t>
+    <t>NaturalGas</t>
   </si>
   <si>
     <t>Soybean</t>
@@ -106,6 +106,9 @@
     <t>Gold</t>
   </si>
   <si>
+    <t>Ethereum</t>
+  </si>
+  <si>
     <t>Southkorea</t>
   </si>
   <si>
@@ -113,6 +116,9 @@
   </si>
   <si>
     <t>Mexico</t>
+  </si>
+  <si>
+    <t>Tehther</t>
   </si>
   <si>
     <t>Russia</t>
@@ -505,15 +511,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -547,13 +553,13 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>6.4291563786112739E-4</v>
+        <v>4.8304055142385797E-4</v>
       </c>
       <c r="C2">
-        <v>1.9880649303973451E-2</v>
+        <v>2.0422206523585951E-2</v>
       </c>
       <c r="D2">
-        <v>1.228713093322398E-3</v>
+        <v>1.360675502368736E-3</v>
       </c>
       <c r="E2">
         <v>-0.15993026567604399</v>
@@ -562,10 +568,10 @@
         <v>0.13022281024270829</v>
       </c>
       <c r="G2">
-        <v>-9.7951629429315658E-3</v>
+        <v>-1.036455869663208E-2</v>
       </c>
       <c r="H2">
-        <v>1.3689235482710871</v>
+        <v>1.257260545190098</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -573,13 +579,13 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>-1.2922890739308209E-4</v>
+        <v>-3.1116379063839459E-4</v>
       </c>
       <c r="C3">
-        <v>1.5517287597128129E-2</v>
+        <v>1.6469670058470439E-2</v>
       </c>
       <c r="D3">
-        <v>1.8431275166097549E-4</v>
+        <v>1.067841228143962E-4</v>
       </c>
       <c r="E3">
         <v>-0.12854533819572289</v>
@@ -588,10 +594,10 @@
         <v>8.8936485781973218E-2</v>
       </c>
       <c r="G3">
-        <v>2.0953543744132629E-2</v>
+        <v>2.2959496288078252E-2</v>
       </c>
       <c r="H3">
-        <v>1.450714907252513</v>
+        <v>1.5292908219206081</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -599,13 +605,13 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>6.9307627494939804E-4</v>
+        <v>1.0804943372392599E-3</v>
       </c>
       <c r="C4">
-        <v>4.1856606030690503E-2</v>
+        <v>4.5277351461191447E-2</v>
       </c>
       <c r="D4">
-        <v>-3.5713290696992578E-4</v>
+        <v>3.4240270918217691E-4</v>
       </c>
       <c r="E4">
         <v>-0.30047976257842501</v>
@@ -614,10 +620,10 @@
         <v>0.4355212407018601</v>
       </c>
       <c r="G4">
-        <v>1.977174054883293E-2</v>
+        <v>3.5583476779334607E-2</v>
       </c>
       <c r="H4">
-        <v>1.342815844242139</v>
+        <v>1.3750363757530599</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,25 +631,25 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>4.4109583137454209E-4</v>
+        <v>7.3111956776918759E-4</v>
       </c>
       <c r="C5">
-        <v>1.614095492849545E-2</v>
+        <v>1.6191306748179441E-2</v>
       </c>
       <c r="D5">
-        <v>7.8435731095716221E-4</v>
+        <v>1.1760739519850461E-3</v>
       </c>
       <c r="E5">
         <v>-9.6032648614778005E-2</v>
       </c>
       <c r="F5">
-        <v>7.6889340761719716E-2</v>
+        <v>7.2748322082193617E-2</v>
       </c>
       <c r="G5">
-        <v>-6.4504818187804208E-2</v>
+        <v>-6.4571424820272477E-2</v>
       </c>
       <c r="H5">
-        <v>1.4156451595634061</v>
+        <v>1.374273709118129</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -651,25 +657,25 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>3.9767905620889161E-4</v>
+        <v>2.1757471112746261E-4</v>
       </c>
       <c r="C6">
-        <v>1.5386495198442681E-2</v>
+        <v>1.48037399288559E-2</v>
       </c>
       <c r="D6">
-        <v>3.5810780858547281E-4</v>
+        <v>3.8138826022926509E-4</v>
       </c>
       <c r="E6">
-        <v>-8.2529328108714495E-2</v>
+        <v>-7.4192312159272689E-2</v>
       </c>
       <c r="F6">
         <v>0.1200715718075074</v>
       </c>
       <c r="G6">
-        <v>3.2334377773556043E-2</v>
+        <v>1.40742384611843E-2</v>
       </c>
       <c r="H6">
-        <v>1.6169321173679649</v>
+        <v>1.578016206147302</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -677,13 +683,13 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>5.3996423229332421E-4</v>
+        <v>6.0236784881574656E-4</v>
       </c>
       <c r="C7">
-        <v>1.3154207050609081E-2</v>
+        <v>1.4203065137333619E-2</v>
       </c>
       <c r="D7">
-        <v>7.7750118615593777E-4</v>
+        <v>1.2405417349583561E-3</v>
       </c>
       <c r="E7">
         <v>-0.10453832109995891</v>
@@ -692,10 +698,10 @@
         <v>8.4002952088621186E-2</v>
       </c>
       <c r="G7">
-        <v>4.202300770608166E-2</v>
+        <v>-3.4522049307325893E-2</v>
       </c>
       <c r="H7">
-        <v>1.3888611574316829</v>
+        <v>1.354151788073279</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -703,13 +709,13 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>-3.097144232422383E-3</v>
+        <v>-5.2913224801868358E-3</v>
       </c>
       <c r="C8">
-        <v>0.135994192365678</v>
+        <v>0.1718285009853856</v>
       </c>
       <c r="D8">
-        <v>1.936356920683391E-3</v>
+        <v>2.202124972804143E-3</v>
       </c>
       <c r="E8">
         <v>-4.5926297537767873</v>
@@ -718,10 +724,10 @@
         <v>0.1081991258551796</v>
       </c>
       <c r="G8">
-        <v>-9.0520017655510099E-2</v>
+        <v>-7.6241159022769373E-2</v>
       </c>
       <c r="H8">
-        <v>1.4367808854469539</v>
+        <v>1.4696348066607869</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -729,25 +735,25 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>-8.777311275377889E-5</v>
+        <v>-1.6170070126910729E-4</v>
       </c>
       <c r="C9">
-        <v>1.7453704370625159E-2</v>
+        <v>1.411320038918913E-2</v>
       </c>
       <c r="D9">
-        <v>5.2571217952479543E-4</v>
+        <v>-6.2108568302576828E-5</v>
       </c>
       <c r="E9">
-        <v>-0.106284707595627</v>
+        <v>-7.1814307724510584E-2</v>
       </c>
       <c r="F9">
-        <v>0.10045306336504289</v>
+        <v>7.5481880201765605E-2</v>
       </c>
       <c r="G9">
-        <v>-5.207946944486818E-2</v>
+        <v>-2.352010970556179E-2</v>
       </c>
       <c r="H9">
-        <v>1.691730993499833</v>
+        <v>1.498410961279222</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -755,13 +761,13 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>4.2476195056362371E-3</v>
+        <v>1.9333823778251509E-3</v>
       </c>
       <c r="C10">
-        <v>5.8782359894833748E-2</v>
+        <v>6.2170271363395438E-2</v>
       </c>
       <c r="D10">
-        <v>2.8668584817119762E-3</v>
+        <v>1.9276925523570301E-3</v>
       </c>
       <c r="E10">
         <v>-0.46473017535485012</v>
@@ -770,10 +776,10 @@
         <v>0.27063751771878591</v>
       </c>
       <c r="G10">
-        <v>0.1038063957261643</v>
+        <v>3.6385275176323971E-2</v>
       </c>
       <c r="H10">
-        <v>1.8436114542407069</v>
+        <v>1.8833039870540731</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -781,13 +787,13 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>3.168425373059601E-4</v>
+        <v>2.1726506607250309E-4</v>
       </c>
       <c r="C11">
-        <v>1.5691293395543648E-2</v>
+        <v>1.6122407180638371E-2</v>
       </c>
       <c r="D11">
-        <v>8.9681522410423042E-4</v>
+        <v>7.1124117500787065E-4</v>
       </c>
       <c r="E11">
         <v>-0.1309834911294932</v>
@@ -796,10 +802,10 @@
         <v>0.16421456444571089</v>
       </c>
       <c r="G11">
-        <v>-8.6352972069750327E-3</v>
+        <v>2.7490006976122389E-2</v>
       </c>
       <c r="H11">
-        <v>1.566487066991447</v>
+        <v>1.466031109924135</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -807,13 +813,13 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>1.8862673319853119E-4</v>
+        <v>7.8995316675032482E-5</v>
       </c>
       <c r="C12">
-        <v>1.7987949396026819E-2</v>
+        <v>1.7287155481237441E-2</v>
       </c>
       <c r="D12">
-        <v>8.4292293336130086E-4</v>
+        <v>1.0452801560383309E-3</v>
       </c>
       <c r="E12">
         <v>-0.1854610663248373</v>
@@ -822,10 +828,10 @@
         <v>0.1159782860158725</v>
       </c>
       <c r="G12">
-        <v>-3.9869505430348347E-2</v>
+        <v>-7.801764312247994E-2</v>
       </c>
       <c r="H12">
-        <v>1.5635923156959659</v>
+        <v>1.5610892419102029</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -833,13 +839,13 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>8.7799019465382923E-5</v>
+        <v>-4.3159533537880947E-5</v>
       </c>
       <c r="C13">
-        <v>1.288502680745753E-2</v>
+        <v>1.3446727882649929E-2</v>
       </c>
       <c r="D13">
-        <v>3.633900059272222E-4</v>
+        <v>2.7145805224026992E-4</v>
       </c>
       <c r="E13">
         <v>-0.1151170613425148</v>
@@ -848,10 +854,10 @@
         <v>0.12125382552797249</v>
       </c>
       <c r="G13">
-        <v>1.122482789143861E-2</v>
+        <v>1.522940082392734E-2</v>
       </c>
       <c r="H13">
-        <v>1.4039457700838089</v>
+        <v>1.3671551798247259</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -859,13 +865,13 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>9.1328157027057094E-4</v>
+        <v>1.244029812180135E-3</v>
       </c>
       <c r="C14">
-        <v>4.2308907853507188E-2</v>
+        <v>4.7346124650061883E-2</v>
       </c>
       <c r="D14">
-        <v>2.374800994116022E-3</v>
+        <v>2.9006985243920091E-3</v>
       </c>
       <c r="E14">
         <v>-0.28179629930639521</v>
@@ -874,10 +880,10 @@
         <v>0.7367530178235584</v>
       </c>
       <c r="G14">
-        <v>-0.11513397737182179</v>
+        <v>-9.6659339330555039E-2</v>
       </c>
       <c r="H14">
-        <v>1.5161191214833429</v>
+        <v>1.5850787190258671</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -885,13 +891,13 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>2.7939916512190448E-4</v>
+        <v>2.8711559839578491E-4</v>
       </c>
       <c r="C15">
-        <v>1.1771010532707271E-2</v>
+        <v>1.3110437925915E-2</v>
       </c>
       <c r="D15">
-        <v>8.5292569224471038E-4</v>
+        <v>7.5768555327559994E-4</v>
       </c>
       <c r="E15">
         <v>-0.1317579985597099</v>
@@ -900,10 +906,10 @@
         <v>9.4088164058783619E-2</v>
       </c>
       <c r="G15">
-        <v>-5.1615837304885538E-2</v>
+        <v>-4.7319044193624453E-3</v>
       </c>
       <c r="H15">
-        <v>1.461663009470425</v>
+        <v>1.4606284524625079</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -911,13 +917,13 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>2.7632991448236192E-4</v>
+        <v>8.4839111695335766E-5</v>
       </c>
       <c r="C16">
-        <v>1.554033383118867E-2</v>
+        <v>1.5802723927694742E-2</v>
       </c>
       <c r="D16">
-        <v>7.6771240372597305E-4</v>
+        <v>5.7513513271789662E-4</v>
       </c>
       <c r="E16">
         <v>-0.13054858703866051</v>
@@ -926,10 +932,10 @@
         <v>0.14970686160126689</v>
       </c>
       <c r="G16">
-        <v>-1.687711781677995E-2</v>
+        <v>1.8067848035785931E-3</v>
       </c>
       <c r="H16">
-        <v>1.6114534569604659</v>
+        <v>1.5779994320982209</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -937,13 +943,13 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>1.951755308797196E-3</v>
+        <v>1.5138978236896891E-3</v>
       </c>
       <c r="C17">
-        <v>3.1552103605129792E-2</v>
+        <v>3.5308498205441359E-2</v>
       </c>
       <c r="D17">
-        <v>1.912507921731255E-3</v>
+        <v>1.868980348497473E-3</v>
       </c>
       <c r="E17">
         <v>-0.37756612018803892</v>
@@ -952,10 +958,10 @@
         <v>0.16851379041827741</v>
       </c>
       <c r="G17">
-        <v>2.7151174614956801E-2</v>
+        <v>-1.1808629433778721E-2</v>
       </c>
       <c r="H17">
-        <v>1.4877762903375309</v>
+        <v>1.4106050605859359</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -963,13 +969,13 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>6.5212655517716124E-4</v>
+        <v>1.2194034131696109E-3</v>
       </c>
       <c r="C18">
-        <v>1.999312739375626E-2</v>
+        <v>2.1265379112407411E-2</v>
       </c>
       <c r="D18">
-        <v>1.3571869974233759E-3</v>
+        <v>1.922094626221504E-3</v>
       </c>
       <c r="E18">
         <v>-0.2057265653202078</v>
@@ -978,10 +984,10 @@
         <v>0.1339103958505872</v>
       </c>
       <c r="G18">
-        <v>-6.1795955488469008E-2</v>
+        <v>-3.2563139561844638E-2</v>
       </c>
       <c r="H18">
-        <v>1.35839218371773</v>
+        <v>1.3685283859815549</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -989,10 +995,10 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>1.6514134413481271E-4</v>
+        <v>2.719931329485087E-4</v>
       </c>
       <c r="C19">
-        <v>1.4296415200231409E-2</v>
+        <v>1.491592731914511E-2</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1001,13 +1007,13 @@
         <v>-0.2009204145294996</v>
       </c>
       <c r="F19">
-        <v>5.4539947946523171E-2</v>
+        <v>4.7447093372394278E-2</v>
       </c>
       <c r="G19">
-        <v>3.9493705548103109E-2</v>
+        <v>0.16154558992285559</v>
       </c>
       <c r="H19">
-        <v>2.1294781255765618</v>
+        <v>3.2688256559461499</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1015,10 +1021,10 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>6.4804182794746127E-4</v>
+        <v>1.4494612591920339E-3</v>
       </c>
       <c r="C20">
-        <v>2.390687018478483E-2</v>
+        <v>2.4961353148912419E-2</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1030,10 +1036,10 @@
         <v>0.2252276481622868</v>
       </c>
       <c r="G20">
-        <v>-3.4669312918279359E-3</v>
+        <v>4.9451987481936847E-2</v>
       </c>
       <c r="H20">
-        <v>1.313464854523307</v>
+        <v>1.405111042272472</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1041,13 +1047,13 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>2.8689530258917638E-4</v>
+        <v>4.510802611599478E-4</v>
       </c>
       <c r="C21">
-        <v>1.147740180107438E-2</v>
+        <v>1.181331735697087E-2</v>
       </c>
       <c r="D21">
-        <v>3.8183038284156368E-4</v>
+        <v>5.3654856223106506E-4</v>
       </c>
       <c r="E21">
         <v>-5.1069383901130472E-2</v>
@@ -1056,10 +1062,10 @@
         <v>0.1097401996827569</v>
       </c>
       <c r="G21">
-        <v>3.9568332716219637E-2</v>
+        <v>5.2835926696156582E-2</v>
       </c>
       <c r="H21">
-        <v>1.507395719439995</v>
+        <v>1.5099550271627471</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1067,25 +1073,25 @@
         <v>28</v>
       </c>
       <c r="B22">
-        <v>2.6694017852327197E-4</v>
+        <v>2.4151700762201889E-3</v>
       </c>
       <c r="C22">
-        <v>1.267551669990183E-2</v>
+        <v>7.9071529143920669E-2</v>
       </c>
       <c r="D22">
-        <v>6.493096308655133E-4</v>
+        <v>1.492403001892129E-3</v>
       </c>
       <c r="E22">
-        <v>-8.7669717954606874E-2</v>
+        <v>-0.55073174413121784</v>
       </c>
       <c r="F22">
-        <v>0.14568249246448681</v>
+        <v>0.32497054552207327</v>
       </c>
       <c r="G22">
-        <v>-2.6806533993861011E-2</v>
+        <v>7.6682003214706071E-2</v>
       </c>
       <c r="H22">
-        <v>1.6666184712153289</v>
+        <v>1.653084038250761</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1093,25 +1099,25 @@
         <v>29</v>
       </c>
       <c r="B23">
-        <v>2.1426519002410761E-4</v>
+        <v>1.3058730819595251E-5</v>
       </c>
       <c r="C23">
-        <v>2.3745949189304501E-2</v>
+        <v>1.460929575752308E-2</v>
       </c>
       <c r="D23">
-        <v>-7.713973517620154E-4</v>
+        <v>7.8666551698924891E-4</v>
       </c>
       <c r="E23">
-        <v>-9.0666084661122248E-2</v>
+        <v>-8.7669717954606874E-2</v>
       </c>
       <c r="F23">
-        <v>0.20961677501600781</v>
+        <v>0.14568249246448681</v>
       </c>
       <c r="G23">
-        <v>2.424096449397363E-2</v>
+        <v>-5.2966219299803191E-2</v>
       </c>
       <c r="H23">
-        <v>1.30449133333454</v>
+        <v>1.5336515701112849</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1119,25 +1125,25 @@
         <v>30</v>
       </c>
       <c r="B24">
-        <v>1.633750992300962E-4</v>
+        <v>3.8504117995412932E-4</v>
       </c>
       <c r="C24">
-        <v>1.1822394753171921E-2</v>
+        <v>2.2365801416451961E-2</v>
       </c>
       <c r="D24">
-        <v>7.6210148564292979E-5</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>-6.7724656807788719E-2</v>
+        <v>-7.5670361506415151E-2</v>
       </c>
       <c r="F24">
-        <v>5.3358431674180203E-2</v>
+        <v>0.20961677501600781</v>
       </c>
       <c r="G24">
-        <v>4.3033475798792721E-2</v>
+        <v>-1.3784849987351159E-2</v>
       </c>
       <c r="H24">
-        <v>1.4047033797279711</v>
+        <v>1.2646956442320809</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1145,25 +1151,25 @@
         <v>31</v>
       </c>
       <c r="B25">
-        <v>3.0319122607806877E-4</v>
+        <v>3.7589637523131212E-5</v>
       </c>
       <c r="C25">
-        <v>2.0193004205695999E-2</v>
+        <v>1.301362000735776E-2</v>
       </c>
       <c r="D25">
-        <v>7.3266211479383614E-4</v>
+        <v>-1.568137249838841E-4</v>
       </c>
       <c r="E25">
-        <v>-0.40467437019784919</v>
+        <v>-6.7724656807788719E-2</v>
       </c>
       <c r="F25">
-        <v>0.18261945405023641</v>
+        <v>5.3358431674180203E-2</v>
       </c>
       <c r="G25">
-        <v>2.09776731479367E-2</v>
+        <v>4.3656162520373937E-2</v>
       </c>
       <c r="H25">
-        <v>1.3112489957093729</v>
+        <v>1.357568990205434</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1171,25 +1177,77 @@
         <v>32</v>
       </c>
       <c r="B26">
-        <v>5.9584862199777344E-4</v>
+        <v>-6.5356340833683287E-6</v>
       </c>
       <c r="C26">
-        <v>1.3122969509003501E-2</v>
+        <v>5.4508079336273423E-3</v>
       </c>
       <c r="D26">
-        <v>9.957057144278636E-4</v>
+        <v>-4.5497760382377053E-5</v>
       </c>
       <c r="E26">
+        <v>-5.2569703281064813E-2</v>
+      </c>
+      <c r="F26">
+        <v>5.3393347829450218E-2</v>
+      </c>
+      <c r="G26">
+        <v>-4.2615520338345383E-2</v>
+      </c>
+      <c r="H26">
+        <v>2.4380424533751128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27">
+        <v>4.9670859439528568E-5</v>
+      </c>
+      <c r="C27">
+        <v>2.3453049587518589E-2</v>
+      </c>
+      <c r="D27">
+        <v>1.060309450344743E-3</v>
+      </c>
+      <c r="E27">
+        <v>-0.40467437019784919</v>
+      </c>
+      <c r="F27">
+        <v>0.18261945405023641</v>
+      </c>
+      <c r="G27">
+        <v>-3.5084951284693362E-2</v>
+      </c>
+      <c r="H27">
+        <v>1.31514876552308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28">
+        <v>6.1548055460312011E-4</v>
+      </c>
+      <c r="C28">
+        <v>1.4787046361160971E-2</v>
+      </c>
+      <c r="D28">
+        <v>1.1478884345348379E-3</v>
+      </c>
+      <c r="E28">
         <v>-9.9944852300803078E-2</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <v>8.8808406952074925E-2</v>
       </c>
-      <c r="G26">
-        <v>5.7899481914231658E-2</v>
-      </c>
-      <c r="H26">
-        <v>1.6509950343277391</v>
+      <c r="G28">
+        <v>2.9557928680021821E-2</v>
+      </c>
+      <c r="H28">
+        <v>1.610515751422682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>